<commit_message>
change the data type
</commit_message>
<xml_diff>
--- a/anlysis/2022-05-16回测-50.xlsx
+++ b/anlysis/2022-05-16回测-50.xlsx
@@ -40,304 +40,304 @@
     <t>证券代码</t>
   </si>
   <si>
-    <t>000001.SZ</t>
-  </si>
-  <si>
-    <t>600714.SH</t>
-  </si>
-  <si>
-    <t>600712.SH</t>
-  </si>
-  <si>
-    <t>600711.SH</t>
-  </si>
-  <si>
-    <t>600710.SH</t>
-  </si>
-  <si>
-    <t>600708.SH</t>
-  </si>
-  <si>
-    <t>600707.SH</t>
-  </si>
-  <si>
-    <t>600706.SH</t>
-  </si>
-  <si>
-    <t>600705.SH</t>
-  </si>
-  <si>
-    <t>600704.SH</t>
-  </si>
-  <si>
-    <t>600703.SH</t>
-  </si>
-  <si>
-    <t>600702.SH</t>
-  </si>
-  <si>
-    <t>600699.SH</t>
-  </si>
-  <si>
-    <t>600698.SH</t>
-  </si>
-  <si>
-    <t>600697.SH</t>
-  </si>
-  <si>
-    <t>600696.SH</t>
-  </si>
-  <si>
-    <t>600695.SH</t>
-  </si>
-  <si>
-    <t>600713.SH</t>
-  </si>
-  <si>
-    <t>600715.SH</t>
-  </si>
-  <si>
-    <t>600693.SH</t>
-  </si>
-  <si>
-    <t>600716.SH</t>
-  </si>
-  <si>
-    <t>600732.SH</t>
-  </si>
-  <si>
-    <t>600731.SH</t>
-  </si>
-  <si>
-    <t>600730.SH</t>
-  </si>
-  <si>
-    <t>600729.SH</t>
-  </si>
-  <si>
-    <t>600728.SH</t>
-  </si>
-  <si>
-    <t>600727.SH</t>
-  </si>
-  <si>
-    <t>600726.SH</t>
-  </si>
-  <si>
-    <t>600725.SH</t>
-  </si>
-  <si>
-    <t>600724.SH</t>
-  </si>
-  <si>
-    <t>600722.SH</t>
-  </si>
-  <si>
-    <t>600721.SH</t>
-  </si>
-  <si>
-    <t>600720.SH</t>
-  </si>
-  <si>
-    <t>600719.SH</t>
-  </si>
-  <si>
-    <t>600718.SH</t>
-  </si>
-  <si>
-    <t>600717.SH</t>
-  </si>
-  <si>
-    <t>600694.SH</t>
-  </si>
-  <si>
-    <t>600692.SH</t>
-  </si>
-  <si>
-    <t>600469.SH</t>
-  </si>
-  <si>
-    <t>600667.SH</t>
-  </si>
-  <si>
-    <t>600665.SH</t>
-  </si>
-  <si>
-    <t>600664.SH</t>
-  </si>
-  <si>
-    <t>600663.SH</t>
-  </si>
-  <si>
-    <t>600662.SH</t>
-  </si>
-  <si>
-    <t>600661.SH</t>
-  </si>
-  <si>
-    <t>600660.SH</t>
-  </si>
-  <si>
-    <t>600658.SH</t>
-  </si>
-  <si>
-    <t>600657.SH</t>
-  </si>
-  <si>
-    <t>600655.SH</t>
-  </si>
-  <si>
-    <t>600654.SH</t>
-  </si>
-  <si>
-    <t>平安银行</t>
-  </si>
-  <si>
-    <t>金瑞矿业</t>
-  </si>
-  <si>
-    <t>南宁百货</t>
-  </si>
-  <si>
-    <t>盛屯矿业</t>
-  </si>
-  <si>
-    <t>苏美达</t>
-  </si>
-  <si>
-    <t>光明地产</t>
-  </si>
-  <si>
-    <t>彩虹股份</t>
-  </si>
-  <si>
-    <t>曲江文旅</t>
-  </si>
-  <si>
-    <t>中航产融</t>
-  </si>
-  <si>
-    <t>物产中大</t>
-  </si>
-  <si>
-    <t>三安光电</t>
-  </si>
-  <si>
-    <t>舍得酒业</t>
-  </si>
-  <si>
-    <t>均胜电子</t>
-  </si>
-  <si>
-    <t>湖南天雁</t>
-  </si>
-  <si>
-    <t>欧亚集团</t>
-  </si>
-  <si>
-    <t>岩石股份</t>
-  </si>
-  <si>
-    <t>退市绿庭</t>
-  </si>
-  <si>
-    <t>南京医药</t>
-  </si>
-  <si>
-    <t>文投控股</t>
-  </si>
-  <si>
-    <t>东百集团</t>
-  </si>
-  <si>
-    <t>凤凰股份</t>
-  </si>
-  <si>
-    <t>爱旭股份</t>
-  </si>
-  <si>
-    <t>湖南海利</t>
-  </si>
-  <si>
-    <t>中国高科</t>
-  </si>
-  <si>
-    <t>重庆百货</t>
-  </si>
-  <si>
-    <t>佳都科技</t>
-  </si>
-  <si>
-    <t>鲁北化工</t>
-  </si>
-  <si>
-    <t>*ST华源</t>
-  </si>
-  <si>
-    <t>云维股份</t>
-  </si>
-  <si>
-    <t>宁波富达</t>
-  </si>
-  <si>
-    <t>金牛化工</t>
-  </si>
-  <si>
-    <t>百花村</t>
-  </si>
-  <si>
-    <t>祁连山</t>
-  </si>
-  <si>
-    <t>ST热电</t>
-  </si>
-  <si>
-    <t>东软集团</t>
-  </si>
-  <si>
-    <t>天津港</t>
-  </si>
-  <si>
-    <t>大商股份</t>
-  </si>
-  <si>
-    <t>亚通股份</t>
-  </si>
-  <si>
-    <t>风神股份</t>
-  </si>
-  <si>
-    <t>太极实业</t>
-  </si>
-  <si>
-    <t>天地源</t>
-  </si>
-  <si>
-    <t>哈药股份</t>
-  </si>
-  <si>
-    <t>陆家嘴</t>
-  </si>
-  <si>
-    <t>外服控股</t>
-  </si>
-  <si>
-    <t>昂立教育</t>
-  </si>
-  <si>
-    <t>福耀玻璃</t>
-  </si>
-  <si>
-    <t>电子城</t>
-  </si>
-  <si>
-    <t>信达地产</t>
-  </si>
-  <si>
-    <t>豫园股份</t>
-  </si>
-  <si>
-    <t>*ST中安</t>
+    <t>000004.SZ</t>
+  </si>
+  <si>
+    <t>600814.SH</t>
+  </si>
+  <si>
+    <t>600792.SH</t>
+  </si>
+  <si>
+    <t>600794.SH</t>
+  </si>
+  <si>
+    <t>600796.SH</t>
+  </si>
+  <si>
+    <t>600797.SH</t>
+  </si>
+  <si>
+    <t>600798.SH</t>
+  </si>
+  <si>
+    <t>600800.SH</t>
+  </si>
+  <si>
+    <t>600801.SH</t>
+  </si>
+  <si>
+    <t>600802.SH</t>
+  </si>
+  <si>
+    <t>600805.SH</t>
+  </si>
+  <si>
+    <t>600808.SH</t>
+  </si>
+  <si>
+    <t>600809.SH</t>
+  </si>
+  <si>
+    <t>600811.SH</t>
+  </si>
+  <si>
+    <t>600815.SH</t>
+  </si>
+  <si>
+    <t>600789.SH</t>
+  </si>
+  <si>
+    <t>600817.SH</t>
+  </si>
+  <si>
+    <t>600818.SH</t>
+  </si>
+  <si>
+    <t>600819.SH</t>
+  </si>
+  <si>
+    <t>600822.SH</t>
+  </si>
+  <si>
+    <t>600824.SH</t>
+  </si>
+  <si>
+    <t>600825.SH</t>
+  </si>
+  <si>
+    <t>600826.SH</t>
+  </si>
+  <si>
+    <t>600830.SH</t>
+  </si>
+  <si>
+    <t>600833.SH</t>
+  </si>
+  <si>
+    <t>600834.SH</t>
+  </si>
+  <si>
+    <t>600836.SH</t>
+  </si>
+  <si>
+    <t>600838.SH</t>
+  </si>
+  <si>
+    <t>600790.SH</t>
+  </si>
+  <si>
+    <t>600787.SH</t>
+  </si>
+  <si>
+    <t>600513.SH</t>
+  </si>
+  <si>
+    <t>600765.SH</t>
+  </si>
+  <si>
+    <t>600742.SH</t>
+  </si>
+  <si>
+    <t>600745.SH</t>
+  </si>
+  <si>
+    <t>600746.SH</t>
+  </si>
+  <si>
+    <t>600749.SH</t>
+  </si>
+  <si>
+    <t>600750.SH</t>
+  </si>
+  <si>
+    <t>600751.SH</t>
+  </si>
+  <si>
+    <t>600753.SH</t>
+  </si>
+  <si>
+    <t>600756.SH</t>
+  </si>
+  <si>
+    <t>600757.SH</t>
+  </si>
+  <si>
+    <t>600761.SH</t>
+  </si>
+  <si>
+    <t>600763.SH</t>
+  </si>
+  <si>
+    <t>600764.SH</t>
+  </si>
+  <si>
+    <t>600766.SH</t>
+  </si>
+  <si>
+    <t>600784.SH</t>
+  </si>
+  <si>
+    <t>600767.SH</t>
+  </si>
+  <si>
+    <t>600768.SH</t>
+  </si>
+  <si>
+    <t>600770.SH</t>
+  </si>
+  <si>
+    <t>600771.SH</t>
+  </si>
+  <si>
+    <t>ST国华</t>
+  </si>
+  <si>
+    <t>杭州解百</t>
+  </si>
+  <si>
+    <t>云煤能源</t>
+  </si>
+  <si>
+    <t>保税科技</t>
+  </si>
+  <si>
+    <t>钱江生化</t>
+  </si>
+  <si>
+    <t>浙大网新</t>
+  </si>
+  <si>
+    <t>宁波海运</t>
+  </si>
+  <si>
+    <t>渤海化学</t>
+  </si>
+  <si>
+    <t>华新水泥</t>
+  </si>
+  <si>
+    <t>福建水泥</t>
+  </si>
+  <si>
+    <t>悦达投资</t>
+  </si>
+  <si>
+    <t>马钢股份</t>
+  </si>
+  <si>
+    <t>山西汾酒</t>
+  </si>
+  <si>
+    <t>东方集团</t>
+  </si>
+  <si>
+    <t>厦工股份</t>
+  </si>
+  <si>
+    <t>鲁抗医药</t>
+  </si>
+  <si>
+    <t>宇通重工</t>
+  </si>
+  <si>
+    <t>中路股份</t>
+  </si>
+  <si>
+    <t>耀皮玻璃</t>
+  </si>
+  <si>
+    <t>上海物贸</t>
+  </si>
+  <si>
+    <t>益民集团</t>
+  </si>
+  <si>
+    <t>新华传媒</t>
+  </si>
+  <si>
+    <t>兰生股份</t>
+  </si>
+  <si>
+    <t>香溢融通</t>
+  </si>
+  <si>
+    <t>第一医药</t>
+  </si>
+  <si>
+    <t>申通地铁</t>
+  </si>
+  <si>
+    <t>上海易连</t>
+  </si>
+  <si>
+    <t>上海九百</t>
+  </si>
+  <si>
+    <t>轻纺城</t>
+  </si>
+  <si>
+    <t>中储股份</t>
+  </si>
+  <si>
+    <t>联环药业</t>
+  </si>
+  <si>
+    <t>中航重机</t>
+  </si>
+  <si>
+    <t>一汽富维</t>
+  </si>
+  <si>
+    <t>闻泰科技</t>
+  </si>
+  <si>
+    <t>江苏索普</t>
+  </si>
+  <si>
+    <t>西藏旅游</t>
+  </si>
+  <si>
+    <t>江中药业</t>
+  </si>
+  <si>
+    <t>海航科技</t>
+  </si>
+  <si>
+    <t>东方银星</t>
+  </si>
+  <si>
+    <t>浪潮软件</t>
+  </si>
+  <si>
+    <t>长江传媒</t>
+  </si>
+  <si>
+    <t>安徽合力</t>
+  </si>
+  <si>
+    <t>通策医疗</t>
+  </si>
+  <si>
+    <t>中国海防</t>
+  </si>
+  <si>
+    <t>*ST园城</t>
+  </si>
+  <si>
+    <t>鲁银投资</t>
+  </si>
+  <si>
+    <t>*ST运盛</t>
+  </si>
+  <si>
+    <t>宁波富邦</t>
+  </si>
+  <si>
+    <t>综艺股份</t>
+  </si>
+  <si>
+    <t>广誉远</t>
   </si>
   <si>
     <t>nan%</t>
@@ -750,7 +750,7 @@
         <v>109</v>
       </c>
       <c r="F2">
-        <v>14.41</v>
+        <v>8.83</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -770,7 +770,7 @@
         <v>109</v>
       </c>
       <c r="F3">
-        <v>12.46</v>
+        <v>7.1</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -790,7 +790,7 @@
         <v>109</v>
       </c>
       <c r="F4">
-        <v>4.28</v>
+        <v>3.95</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -810,7 +810,7 @@
         <v>109</v>
       </c>
       <c r="F5">
-        <v>7.19</v>
+        <v>3.28</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -830,7 +830,7 @@
         <v>109</v>
       </c>
       <c r="F6">
-        <v>5.72</v>
+        <v>5.21</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -850,7 +850,7 @@
         <v>109</v>
       </c>
       <c r="F7">
-        <v>2.78</v>
+        <v>5.41</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -870,7 +870,7 @@
         <v>109</v>
       </c>
       <c r="F8">
-        <v>4.21</v>
+        <v>4.19</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -890,7 +890,7 @@
         <v>109</v>
       </c>
       <c r="F9">
-        <v>11.03</v>
+        <v>3.95</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -910,7 +910,7 @@
         <v>109</v>
       </c>
       <c r="F10">
-        <v>3.28</v>
+        <v>21.47</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -930,7 +930,7 @@
         <v>109</v>
       </c>
       <c r="F11">
-        <v>5.03</v>
+        <v>6.39</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -950,7 +950,7 @@
         <v>109</v>
       </c>
       <c r="F12">
-        <v>20.18</v>
+        <v>4.83</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -970,7 +970,7 @@
         <v>109</v>
       </c>
       <c r="F13">
-        <v>144.68</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -990,7 +990,7 @@
         <v>109</v>
       </c>
       <c r="F14">
-        <v>11.35</v>
+        <v>254.95</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -1010,7 +1010,7 @@
         <v>109</v>
       </c>
       <c r="F15">
-        <v>5.17</v>
+        <v>2.89</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -1030,7 +1030,7 @@
         <v>109</v>
       </c>
       <c r="F16">
-        <v>14.41</v>
+        <v>2.9</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1050,7 +1050,7 @@
         <v>109</v>
       </c>
       <c r="F17">
-        <v>25.8</v>
+        <v>7.04</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1070,7 +1070,7 @@
         <v>109</v>
       </c>
       <c r="F18">
-        <v>1.7</v>
+        <v>7.95</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1090,7 +1090,7 @@
         <v>109</v>
       </c>
       <c r="F19">
-        <v>4.85</v>
+        <v>17.51</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1110,7 +1110,7 @@
         <v>109</v>
       </c>
       <c r="F20">
-        <v>2.16</v>
+        <v>4.84</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1130,7 +1130,7 @@
         <v>109</v>
       </c>
       <c r="F21">
-        <v>4.47</v>
+        <v>8.57</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1150,7 +1150,7 @@
         <v>109</v>
       </c>
       <c r="F22">
-        <v>5.32</v>
+        <v>4.16</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1170,7 +1170,7 @@
         <v>109</v>
       </c>
       <c r="F23">
-        <v>19.6</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1190,7 +1190,7 @@
         <v>109</v>
       </c>
       <c r="F24">
-        <v>7.47</v>
+        <v>7.55</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1210,7 +1210,7 @@
         <v>109</v>
       </c>
       <c r="F25">
-        <v>5.14</v>
+        <v>5.29</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1230,7 +1230,7 @@
         <v>109</v>
       </c>
       <c r="F26">
-        <v>22.28</v>
+        <v>9.82</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1250,7 +1250,7 @@
         <v>109</v>
       </c>
       <c r="F27">
-        <v>6.27</v>
+        <v>8.48</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1270,7 +1270,7 @@
         <v>109</v>
       </c>
       <c r="F28">
-        <v>8.359999999999999</v>
+        <v>5.79</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1290,7 +1290,7 @@
         <v>109</v>
       </c>
       <c r="F29">
-        <v>2.1</v>
+        <v>10.1</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1310,7 +1310,7 @@
         <v>109</v>
       </c>
       <c r="F30">
-        <v>3.54</v>
+        <v>4.08</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1330,7 +1330,7 @@
         <v>109</v>
       </c>
       <c r="F31">
-        <v>4.89</v>
+        <v>5.72</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1350,7 +1350,7 @@
         <v>109</v>
       </c>
       <c r="F32">
-        <v>5.3</v>
+        <v>9.949999999999999</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1370,7 +1370,7 @@
         <v>109</v>
       </c>
       <c r="F33">
-        <v>7.2</v>
+        <v>40.03</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1390,7 +1390,7 @@
         <v>109</v>
       </c>
       <c r="F34">
-        <v>14.25</v>
+        <v>8.6</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1410,7 +1410,7 @@
         <v>109</v>
       </c>
       <c r="F35">
-        <v>3.89</v>
+        <v>67.54000000000001</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1430,7 +1430,7 @@
         <v>109</v>
       </c>
       <c r="F36">
-        <v>9.73</v>
+        <v>10.7</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1450,7 +1450,7 @@
         <v>109</v>
       </c>
       <c r="F37">
-        <v>4.09</v>
+        <v>12.18</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1470,7 +1470,7 @@
         <v>109</v>
       </c>
       <c r="F38">
-        <v>21.83</v>
+        <v>13.96</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1490,7 +1490,7 @@
         <v>109</v>
       </c>
       <c r="F39">
-        <v>6.3</v>
+        <v>2.73</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1510,7 +1510,7 @@
         <v>109</v>
       </c>
       <c r="F40">
-        <v>3.88</v>
+        <v>11.67</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1530,7 +1530,7 @@
         <v>109</v>
       </c>
       <c r="F41">
-        <v>7.1</v>
+        <v>12.36</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1550,7 +1550,7 @@
         <v>109</v>
       </c>
       <c r="F42">
-        <v>3.81</v>
+        <v>5.38</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1570,7 +1570,7 @@
         <v>109</v>
       </c>
       <c r="F43">
-        <v>3</v>
+        <v>9.869999999999999</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1590,7 +1590,7 @@
         <v>109</v>
       </c>
       <c r="F44">
-        <v>10.8</v>
+        <v>125.88</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1610,7 +1610,7 @@
         <v>109</v>
       </c>
       <c r="F45">
-        <v>5.78</v>
+        <v>22.37</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -1630,7 +1630,7 @@
         <v>109</v>
       </c>
       <c r="F46">
-        <v>8.43</v>
+        <v>6</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -1650,7 +1650,7 @@
         <v>109</v>
       </c>
       <c r="F47">
-        <v>37.6</v>
+        <v>6.15</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -1670,7 +1670,7 @@
         <v>109</v>
       </c>
       <c r="F48">
-        <v>4.32</v>
+        <v>4.02</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -1690,7 +1690,7 @@
         <v>109</v>
       </c>
       <c r="F49">
-        <v>6.91</v>
+        <v>8.16</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -1710,7 +1710,7 @@
         <v>109</v>
       </c>
       <c r="F50">
-        <v>9.9</v>
+        <v>10.03</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -1730,7 +1730,7 @@
         <v>109</v>
       </c>
       <c r="F51">
-        <v>1.92</v>
+        <v>29.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>